<commit_message>
fixed final numbers count
</commit_message>
<xml_diff>
--- a/evaluations/manual/pl-marker_ace05_bert_RE_jun17_eval.xlsx
+++ b/evaluations/manual/pl-marker_ace05_bert_RE_jun17_eval.xlsx
@@ -18798,8 +18798,8 @@
         <v>21</v>
       </c>
       <c r="Q2" s="2">
-        <f>AVERAGE(J2:J19)</f>
-        <v>1</v>
+        <f>AVERAGE(J2:J1000)</f>
+        <v>0.996031746</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>22</v>
@@ -18854,8 +18854,8 @@
         <v>29</v>
       </c>
       <c r="Q3" s="2">
-        <f> AVERAGE(K2:K19)</f>
-        <v>0.9444444444</v>
+        <f> AVERAGE(K2:K1000)</f>
+        <v>0.9920634921</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>30</v>
@@ -18912,7 +18912,7 @@
         <v>37</v>
       </c>
       <c r="Q4" s="2">
-        <f>AVERAGE(L2:L19)</f>
+        <f>AVERAGE(L2:L1000)</f>
         <v>1</v>
       </c>
       <c r="S4" s="2" t="s">
@@ -18968,7 +18968,7 @@
         <v>44</v>
       </c>
       <c r="Q5" s="2">
-        <f>SUM(M2:M19)</f>
+        <f>SUM(M2:M1000)</f>
         <v>0</v>
       </c>
       <c r="S5" s="2" t="s">

</xml_diff>